<commit_message>
added data for 2021 for most univs
</commit_message>
<xml_diff>
--- a/data/ki/original_data/ki_2021_q2.xlsx
+++ b/data/ki/original_data/ki_2021_q2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilla/Documents/repos/openapc-se/data/ki/original_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEF7CA0D-4AD3-B54D-A7F7-0FE632F38916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1342EF10-C5D4-524A-BC98-5612A1DCAFA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="500" windowWidth="26980" windowHeight="14860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26980" windowHeight="14860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="134">
   <si>
     <t>institution</t>
   </si>
@@ -302,9 +302,6 @@
   </si>
   <si>
     <t>10.3389/fmicb.2021.667718</t>
-  </si>
-  <si>
-    <t>10.3389/fmicb.2021.696522</t>
   </si>
   <si>
     <t>10.3389/fnagi.2021.644611</t>
@@ -810,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K132"/>
+  <dimension ref="A1:K131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="144" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="144" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:XFD74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -869,7 +866,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B2" s="2">
         <v>2021</v>
@@ -886,7 +883,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B3" s="2">
         <v>2021</v>
@@ -903,7 +900,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B4" s="2">
         <v>2021</v>
@@ -920,7 +917,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B5" s="2">
         <v>2021</v>
@@ -937,7 +934,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B6" s="2">
         <v>2021</v>
@@ -954,7 +951,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B7" s="2">
         <v>2021</v>
@@ -971,7 +968,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B8" s="2">
         <v>2021</v>
@@ -988,7 +985,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B9" s="2">
         <v>2021</v>
@@ -1005,7 +1002,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B10" s="2">
         <v>2021</v>
@@ -1022,7 +1019,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B11" s="2">
         <v>2021</v>
@@ -1039,7 +1036,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B12" s="2">
         <v>2021</v>
@@ -1056,7 +1053,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B13" s="2">
         <v>2021</v>
@@ -1073,7 +1070,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B14" s="2">
         <v>2021</v>
@@ -1090,7 +1087,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B15" s="2">
         <v>2021</v>
@@ -1107,7 +1104,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B16" s="2">
         <v>2021</v>
@@ -1124,7 +1121,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B17" s="2">
         <v>2021</v>
@@ -1141,7 +1138,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B18" s="2">
         <v>2021</v>
@@ -1158,7 +1155,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B19" s="2">
         <v>2021</v>
@@ -1175,7 +1172,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B20" s="2">
         <v>2021</v>
@@ -1192,7 +1189,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B21" s="2">
         <v>2021</v>
@@ -1209,7 +1206,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B22" s="2">
         <v>2021</v>
@@ -1226,7 +1223,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B23" s="2">
         <v>2021</v>
@@ -1243,7 +1240,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B24" s="2">
         <v>2021</v>
@@ -1260,7 +1257,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B25" s="2">
         <v>2021</v>
@@ -1277,7 +1274,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B26" s="2">
         <v>2021</v>
@@ -1294,7 +1291,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B27" s="2">
         <v>2021</v>
@@ -1311,7 +1308,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B28" s="2">
         <v>2021</v>
@@ -1328,7 +1325,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B29" s="2">
         <v>2021</v>
@@ -1345,7 +1342,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B30" s="2">
         <v>2021</v>
@@ -1362,7 +1359,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B31" s="2">
         <v>2021</v>
@@ -1379,7 +1376,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B32" s="2">
         <v>2021</v>
@@ -1396,7 +1393,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B33" s="2">
         <v>2021</v>
@@ -1413,7 +1410,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B34" s="2">
         <v>2021</v>
@@ -1430,7 +1427,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B35" s="2">
         <v>2021</v>
@@ -1447,7 +1444,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B36" s="2">
         <v>2021</v>
@@ -1464,7 +1461,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B37" s="2">
         <v>2021</v>
@@ -1481,7 +1478,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B38" s="2">
         <v>2021</v>
@@ -1498,7 +1495,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B39" s="2">
         <v>2021</v>
@@ -1515,7 +1512,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B40" s="2">
         <v>2021</v>
@@ -1532,7 +1529,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B41" s="2">
         <v>2021</v>
@@ -1549,7 +1546,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B42" s="2">
         <v>2021</v>
@@ -1566,7 +1563,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B43" s="2">
         <v>2021</v>
@@ -1583,7 +1580,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B44" s="2">
         <v>2021</v>
@@ -1600,7 +1597,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B45" s="2">
         <v>2021</v>
@@ -1617,7 +1614,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B46" s="2">
         <v>2021</v>
@@ -1634,7 +1631,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B47" s="2">
         <v>2021</v>
@@ -1651,7 +1648,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B48" s="2">
         <v>2021</v>
@@ -1668,7 +1665,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B49" s="2">
         <v>2021</v>
@@ -1685,7 +1682,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B50" s="2">
         <v>2021</v>
@@ -1702,7 +1699,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B51" s="2">
         <v>2021</v>
@@ -1719,7 +1716,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B52" s="2">
         <v>2021</v>
@@ -1736,7 +1733,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B53" s="2">
         <v>2021</v>
@@ -1753,7 +1750,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B54" s="2">
         <v>2021</v>
@@ -1770,7 +1767,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B55" s="2">
         <v>2021</v>
@@ -1787,7 +1784,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B56" s="2">
         <v>2021</v>
@@ -1804,7 +1801,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B57" s="2">
         <v>2021</v>
@@ -1821,7 +1818,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B58" s="2">
         <v>2021</v>
@@ -1838,7 +1835,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B59" s="2">
         <v>2021</v>
@@ -1855,7 +1852,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B60" s="2">
         <v>2021</v>
@@ -1872,7 +1869,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B61" s="2">
         <v>2021</v>
@@ -1889,7 +1886,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B62" s="2">
         <v>2021</v>
@@ -1906,7 +1903,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B63" s="2">
         <v>2021</v>
@@ -1923,7 +1920,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B64" s="2">
         <v>2021</v>
@@ -1940,7 +1937,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B65" s="2">
         <v>2021</v>
@@ -1957,7 +1954,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B66" s="2">
         <v>2021</v>
@@ -1974,7 +1971,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B67" s="2">
         <v>2021</v>
@@ -1991,7 +1988,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B68" s="2">
         <v>2021</v>
@@ -2008,7 +2005,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B69" s="2">
         <v>2021</v>
@@ -2025,7 +2022,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B70" s="2">
         <v>2021</v>
@@ -2042,7 +2039,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B71" s="2">
         <v>2021</v>
@@ -2059,7 +2056,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B72" s="2">
         <v>2021</v>
@@ -2076,7 +2073,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B73" s="2">
         <v>2021</v>
@@ -2093,13 +2090,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B74" s="2">
         <v>2021</v>
       </c>
       <c r="C74" s="4">
-        <v>24448.42</v>
+        <v>18303.349999999999</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>83</v>
@@ -2110,13 +2107,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B75" s="2">
         <v>2021</v>
       </c>
       <c r="C75" s="4">
-        <v>18303.349999999999</v>
+        <v>24477.63</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>84</v>
@@ -2127,13 +2124,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B76" s="2">
         <v>2021</v>
       </c>
       <c r="C76" s="4">
-        <v>24477.63</v>
+        <v>15402.18</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>85</v>
@@ -2144,13 +2141,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B77" s="2">
         <v>2021</v>
       </c>
       <c r="C77" s="4">
-        <v>15402.18</v>
+        <v>16869.27</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>86</v>
@@ -2161,13 +2158,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B78" s="2">
         <v>2021</v>
       </c>
       <c r="C78" s="4">
-        <v>16869.27</v>
+        <v>15628.99</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>87</v>
@@ -2178,13 +2175,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B79" s="2">
         <v>2021</v>
       </c>
       <c r="C79" s="4">
-        <v>15628.99</v>
+        <v>24748.14</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>88</v>
@@ -2195,13 +2192,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B80" s="2">
         <v>2021</v>
       </c>
       <c r="C80" s="4">
-        <v>24748.14</v>
+        <v>24330.720000000001</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>89</v>
@@ -2212,13 +2209,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B81" s="2">
         <v>2021</v>
       </c>
       <c r="C81" s="4">
-        <v>24330.720000000001</v>
+        <v>25735.51</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>90</v>
@@ -2229,13 +2226,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B82" s="2">
         <v>2021</v>
       </c>
       <c r="C82" s="4">
-        <v>25735.51</v>
+        <v>12539.86</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>91</v>
@@ -2246,13 +2243,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B83" s="2">
         <v>2021</v>
       </c>
       <c r="C83" s="4">
-        <v>12539.86</v>
+        <v>15736.47</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>92</v>
@@ -2263,13 +2260,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B84" s="2">
         <v>2021</v>
       </c>
       <c r="C84" s="4">
-        <v>15736.47</v>
+        <v>24697.11</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>93</v>
@@ -2280,13 +2277,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B85" s="2">
         <v>2021</v>
       </c>
       <c r="C85" s="4">
-        <v>24697.11</v>
+        <v>24591.79</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>94</v>
@@ -2297,13 +2294,13 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B86" s="2">
         <v>2021</v>
       </c>
       <c r="C86" s="4">
-        <v>24591.79</v>
+        <v>24991.52</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>95</v>
@@ -2314,13 +2311,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B87" s="2">
         <v>2021</v>
       </c>
       <c r="C87" s="4">
-        <v>24991.52</v>
+        <v>22319.52</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>96</v>
@@ -2331,13 +2328,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B88" s="2">
         <v>2021</v>
       </c>
       <c r="C88" s="4">
-        <v>22319.52</v>
+        <v>24484.12</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>97</v>
@@ -2348,13 +2345,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B89" s="2">
         <v>2021</v>
       </c>
       <c r="C89" s="4">
-        <v>24484.12</v>
+        <v>6138.88</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>98</v>
@@ -2365,13 +2362,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B90" s="2">
         <v>2021</v>
       </c>
       <c r="C90" s="4">
-        <v>6138.88</v>
+        <v>25441.39</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>99</v>
@@ -2382,13 +2379,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B91" s="2">
         <v>2021</v>
       </c>
       <c r="C91" s="4">
-        <v>25441.39</v>
+        <v>15372.76</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>100</v>
@@ -2399,13 +2396,13 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B92" s="2">
         <v>2021</v>
       </c>
       <c r="C92" s="4">
-        <v>15372.76</v>
+        <v>24762.6</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>101</v>
@@ -2416,13 +2413,13 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B93" s="2">
         <v>2021</v>
       </c>
       <c r="C93" s="4">
-        <v>24762.6</v>
+        <v>4539.83</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>102</v>
@@ -2433,13 +2430,13 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B94" s="2">
         <v>2021</v>
       </c>
       <c r="C94" s="4">
-        <v>4539.83</v>
+        <v>11534.52</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>103</v>
@@ -2450,13 +2447,13 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B95" s="2">
         <v>2021</v>
       </c>
       <c r="C95" s="4">
-        <v>11534.52</v>
+        <v>16302.38</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>104</v>
@@ -2467,13 +2464,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B96" s="2">
         <v>2021</v>
       </c>
       <c r="C96" s="4">
-        <v>16302.38</v>
+        <v>9110.25</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>105</v>
@@ -2484,13 +2481,13 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B97" s="2">
         <v>2021</v>
       </c>
       <c r="C97" s="4">
-        <v>9110.25</v>
+        <v>20133.88</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>106</v>
@@ -2501,13 +2498,13 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B98" s="2">
         <v>2021</v>
       </c>
       <c r="C98" s="4">
-        <v>20133.88</v>
+        <v>19076.32</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>107</v>
@@ -2518,13 +2515,13 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B99" s="2">
         <v>2021</v>
       </c>
       <c r="C99" s="4">
-        <v>19076.32</v>
+        <v>18257.38</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>108</v>
@@ -2535,13 +2532,13 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B100" s="2">
         <v>2021</v>
       </c>
       <c r="C100" s="4">
-        <v>18257.38</v>
+        <v>14663.14</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>109</v>
@@ -2552,13 +2549,13 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B101" s="2">
         <v>2021</v>
       </c>
       <c r="C101" s="4">
-        <v>14663.14</v>
+        <v>21171.61</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>110</v>
@@ -2569,13 +2566,13 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B102" s="2">
         <v>2021</v>
       </c>
       <c r="C102" s="4">
-        <v>21171.61</v>
+        <v>21196.5</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>111</v>
@@ -2586,13 +2583,13 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B103" s="2">
         <v>2021</v>
       </c>
       <c r="C103" s="4">
-        <v>21196.5</v>
+        <v>18958.61</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>112</v>
@@ -2603,13 +2600,13 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B104" s="2">
         <v>2021</v>
       </c>
       <c r="C104" s="4">
-        <v>18958.61</v>
+        <v>18977.240000000002</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>113</v>
@@ -2620,13 +2617,13 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B105" s="2">
         <v>2021</v>
       </c>
       <c r="C105" s="4">
-        <v>18977.240000000002</v>
+        <v>16437.419999999998</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>114</v>
@@ -2637,7 +2634,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B106" s="2">
         <v>2021</v>
@@ -2654,13 +2651,13 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B107" s="2">
         <v>2021</v>
       </c>
       <c r="C107" s="4">
-        <v>16437.419999999998</v>
+        <v>16349.12</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>116</v>
@@ -2671,13 +2668,13 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B108" s="2">
         <v>2021</v>
       </c>
       <c r="C108" s="4">
-        <v>16349.12</v>
+        <v>9585.1200000000008</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>117</v>
@@ -2688,13 +2685,13 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B109" s="2">
         <v>2021</v>
       </c>
       <c r="C109" s="4">
-        <v>9585.1200000000008</v>
+        <v>12300.67</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>118</v>
@@ -2705,13 +2702,13 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B110" s="2">
         <v>2021</v>
       </c>
       <c r="C110" s="4">
-        <v>12300.67</v>
+        <v>13857.04</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>119</v>
@@ -2722,13 +2719,13 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B111" s="2">
         <v>2021</v>
       </c>
       <c r="C111" s="4">
-        <v>13857.04</v>
+        <v>16774.29</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>120</v>
@@ -2739,13 +2736,13 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B112" s="2">
         <v>2021</v>
       </c>
       <c r="C112" s="4">
-        <v>16774.29</v>
+        <v>14620.29</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>121</v>
@@ -2756,13 +2753,13 @@
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B113" s="2">
         <v>2021</v>
       </c>
       <c r="C113" s="4">
-        <v>14620.29</v>
+        <v>12986.49</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>122</v>
@@ -2773,13 +2770,13 @@
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B114" s="2">
         <v>2021</v>
       </c>
       <c r="C114" s="4">
-        <v>12986.49</v>
+        <v>16582.2</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>123</v>
@@ -2790,13 +2787,13 @@
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B115" s="2">
         <v>2021</v>
       </c>
       <c r="C115" s="4">
-        <v>16582.2</v>
+        <v>17415.87</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>124</v>
@@ -2807,13 +2804,13 @@
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B116" s="2">
         <v>2021</v>
       </c>
       <c r="C116" s="4">
-        <v>17415.87</v>
+        <v>10020.77</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>125</v>
@@ -2824,13 +2821,13 @@
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B117" s="2">
         <v>2021</v>
       </c>
       <c r="C117" s="4">
-        <v>10020.77</v>
+        <v>20108.09</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>126</v>
@@ -2841,80 +2838,66 @@
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B118" s="2">
         <v>2021</v>
       </c>
       <c r="C118" s="4">
-        <v>20108.09</v>
+        <v>23307.51</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>127</v>
       </c>
       <c r="E118" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B119" s="2">
         <v>2021</v>
       </c>
       <c r="C119" s="4">
-        <v>23307.51</v>
+        <v>21367.54</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>128</v>
       </c>
       <c r="E119" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B120" s="2">
         <v>2021</v>
       </c>
       <c r="C120" s="4">
-        <v>21367.54</v>
-      </c>
-      <c r="D120" s="2" t="s">
+        <v>2026.86</v>
+      </c>
+      <c r="E120" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F120" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E120" s="2" t="b">
-        <v>0</v>
+      <c r="G120" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J120" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K120" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A121" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B121" s="2">
-        <v>2021</v>
-      </c>
-      <c r="C121" s="4">
-        <v>2026.86</v>
-      </c>
-      <c r="E121" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F121" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="G121" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J121" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="K121" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C121" s="3"/>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C122" s="3"/>
@@ -2945,9 +2928,6 @@
     </row>
     <row r="131" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C131" s="3"/>
-    </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C132" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">

</xml_diff>